<commit_message>
1.Remove `ExcludeFileNames` and `ExcludeSheetNames`. 2.Add `!` Rule For `xlsx` and `sheet` export ignore. 3.Add `ColorToGroupMap` and `GroupFilter` For Column Filter. 4.Improve code robustness. 5.Update README.md.
</commit_message>
<xml_diff>
--- a/testcase/Example.xlsx
+++ b/testcase/Example.xlsx
@@ -1,28 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\excel_tiny_wrapper\testcase\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181363D6-B854-4C59-89D8-CBE270FC8A4B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12615" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
     <sheet name="TestCase" sheetId="2" r:id="rId2"/>
     <sheet name="BoolTest" sheetId="3" r:id="rId3"/>
+    <sheet name="ArrayCase" sheetId="4" r:id="rId4"/>
+    <sheet name="!ExcludeSheet" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -240,6 +236,9 @@
     <t>["2018/12/31 00:00:00"]</t>
   </si>
   <si>
+    <t># Test boolean</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -249,30 +248,263 @@
     <t>bool</t>
   </si>
   <si>
-    <t># Test boolean</t>
+    <t>#Array Test Case</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>int_2</t>
+  </si>
+  <si>
+    <t>int_2_2</t>
+  </si>
+  <si>
+    <t>int_n_2</t>
+  </si>
+  <si>
+    <t>#int_n_n_n</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Error Array Level Less than 3</t>
+  </si>
+  <si>
+    <t>int[2][2]</t>
+  </si>
+  <si>
+    <t>int[][][]</t>
+  </si>
+  <si>
+    <t>[1,2]</t>
+  </si>
+  <si>
+    <t>[[1,1],[2,2]]</t>
+  </si>
+  <si>
+    <t>[3,4]</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf </t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>vsdcv</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>ert</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>fcv</t>
+  </si>
+  <si>
+    <t>erwt</t>
+  </si>
+  <si>
+    <t>cx</t>
+  </si>
+  <si>
+    <t>ertwer</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>wert</t>
+  </si>
+  <si>
+    <t>fas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,8 +517,206 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -294,40 +724,328 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="常规 15" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+  <cellStyles count="51">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="常规 10" xfId="47"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="49" builtinId="52"/>
+    <cellStyle name="常规 15" xfId="50"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -614,42 +1332,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49.2833333333333" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="15" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
-    <col min="18" max="18" width="20.85546875" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="9.425" customWidth="1"/>
+    <col min="5" max="5" width="18.425" customWidth="1"/>
+    <col min="6" max="6" width="11.5666666666667" customWidth="1"/>
+    <col min="7" max="7" width="12.7083333333333" customWidth="1"/>
+    <col min="8" max="8" width="18.425" customWidth="1"/>
+    <col min="9" max="9" width="20.425" customWidth="1"/>
+    <col min="10" max="10" width="21.8583333333333" customWidth="1"/>
+    <col min="11" max="11" width="14.1416666666667" customWidth="1"/>
+    <col min="12" max="12" width="17.425" customWidth="1"/>
+    <col min="13" max="13" width="19.7083333333333" customWidth="1"/>
+    <col min="14" max="15" width="14.8583333333333" customWidth="1"/>
+    <col min="16" max="16" width="17.2833333333333" customWidth="1"/>
+    <col min="17" max="17" width="18.2833333333333" customWidth="1"/>
+    <col min="18" max="18" width="20.8583333333333" customWidth="1"/>
+    <col min="19" max="19" width="13.5666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -708,7 +1426,7 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
@@ -763,71 +1481,71 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="60">
-      <c r="A3" s="6" t="s">
+    <row r="3" ht="54" spans="1:19">
+      <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="75">
-      <c r="A4" s="5">
+    <row r="4" ht="67.5" spans="1:19">
+      <c r="A4" s="4">
         <v>1000001</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D4">
@@ -840,7 +1558,7 @@
         <v>0.1</v>
       </c>
       <c r="G4">
-        <v>1.0001111110000001</v>
+        <v>1.000111111</v>
       </c>
       <c r="H4" t="s">
         <v>51</v>
@@ -851,16 +1569,16 @@
       <c r="K4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="9">
         <v>43415</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="9">
         <v>43415</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="9">
         <v>43415</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="9">
         <v>43415</v>
       </c>
       <c r="P4" t="s">
@@ -870,14 +1588,14 @@
         <v>55</v>
       </c>
       <c r="R4">
-        <v>1123.0123456788999</v>
-      </c>
-      <c r="S4" s="1" t="s">
+        <v>1123.0123456789</v>
+      </c>
+      <c r="S4" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="5">
+    <row r="5" spans="1:18">
+      <c r="A5" s="4">
         <v>1000002</v>
       </c>
       <c r="C5" t="s">
@@ -901,24 +1619,24 @@
       <c r="K5" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="2">
-        <v>43831.499988425901</v>
-      </c>
-      <c r="M5" s="2">
-        <v>43831.499988425901</v>
-      </c>
-      <c r="N5" s="2">
-        <v>43831.499988425901</v>
-      </c>
-      <c r="O5" s="2">
-        <v>43831.499988425901</v>
+      <c r="L5" s="9">
+        <v>43831.4999884259</v>
+      </c>
+      <c r="M5" s="9">
+        <v>43831.4999884259</v>
+      </c>
+      <c r="N5" s="9">
+        <v>43831.4999884259</v>
+      </c>
+      <c r="O5" s="9">
+        <v>43831.4999884259</v>
       </c>
       <c r="R5">
         <v>1.555555555</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="5">
+    <row r="6" spans="1:18">
+      <c r="A6" s="4">
         <v>1000003</v>
       </c>
       <c r="C6" t="s">
@@ -932,23 +1650,25 @@
       </c>
     </row>
     <row r="26" spans="15:15">
-      <c r="O26" s="1"/>
+      <c r="O26" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -1005,22 +1725,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1028,15 +1750,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1079,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:1">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1087,5 +1809,261 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Simplify Array Format Old Format: int[][] [[1,2],[3,4,5]]
New Format:
1,2;3,4,5
"," is the first level separator
";" is the second level separator
"\n" is the third level separator
</commit_message>
<xml_diff>
--- a/testcase/Example.xlsx
+++ b/testcase/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12615" activeTab="4"/>
+    <workbookView windowWidth="23835" windowHeight="12615"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -175,34 +175,28 @@
     <t>123'456'zzz</t>
   </si>
   <si>
-    <t>[100000,1000001]</t>
-  </si>
-  <si>
-    <t>[1,2,43,5,6,76,7]</t>
-  </si>
-  <si>
-    <t>[[1,10],[2,100.10]]</t>
-  </si>
-  <si>
-    <t>["2018/01/01 23:59:59"]</t>
-  </si>
-  <si>
-    <t>["2018/01/01 00:00:00", "2018/01/01 23:59:59"]</t>
-  </si>
-  <si>
-    <t>["line1
+    <t>1000000,100011011</t>
+  </si>
+  <si>
+    <t>1,2,43,5,6,76,7</t>
+  </si>
+  <si>
+    <t>1,10;2,100.10</t>
+  </si>
+  <si>
+    <t>2018/01/01 00:00:00, 2018/01/01 23:59:59</t>
+  </si>
+  <si>
+    <t>line1
 line2
-line3",
-"nextline1
-nextline2"]</t>
+line3,
+nextline1
+nextline2</t>
   </si>
   <si>
     <t>lxjc;s;ldfkjasldfj,;asldfkjsdfakljasdf l;asj;f;a,</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
     <t>A023;_ASDLFKJLJ;,</t>
   </si>
   <si>
@@ -224,16 +218,16 @@
     <t>timestamp[]</t>
   </si>
   <si>
-    <t>[[1,1],[2,2],[3,3]]</t>
+    <t>1,1;2,2;3,3</t>
   </si>
   <si>
     <t>[[1,1,1],[2,2,2]]</t>
   </si>
   <si>
-    <t>[[1.0,0.1],[1,1],[2,2]]</t>
-  </si>
-  <si>
-    <t>["2018/12/31 00:00:00"]</t>
+    <t>1.0,0.1;1,1;2,2</t>
+  </si>
+  <si>
+    <t>2018/12/31 00:00:00,2018/12/31 00:00:00</t>
   </si>
   <si>
     <t># Test boolean</t>
@@ -266,7 +260,7 @@
     <t>int_2</t>
   </si>
   <si>
-    <t>int_2_2</t>
+    <t>#int_2_2</t>
   </si>
   <si>
     <t>int_n_2</t>
@@ -287,13 +281,28 @@
     <t>int[][][]</t>
   </si>
   <si>
-    <t>[1,2]</t>
-  </si>
-  <si>
-    <t>[[1,1],[2,2]]</t>
-  </si>
-  <si>
-    <t>[3,4]</t>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>111,222;333,444</t>
+  </si>
+  <si>
+    <t>11,22</t>
+  </si>
+  <si>
+    <t>222,333;444,555;555,666</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>22,33</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>33,44</t>
   </si>
   <si>
     <t>name</t>
@@ -346,10 +355,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -360,8 +369,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -374,9 +384,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -398,7 +468,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,7 +476,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,54 +497,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,29 +512,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -531,73 +540,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,109 +714,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,50 +731,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -799,6 +764,59 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -813,25 +831,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -840,153 +849,158 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="51">
@@ -1340,8 +1354,8 @@
   <sheetPr/>
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1353,13 +1367,13 @@
     <col min="5" max="5" width="18.425" customWidth="1"/>
     <col min="6" max="6" width="11.5666666666667" customWidth="1"/>
     <col min="7" max="7" width="12.7083333333333" customWidth="1"/>
-    <col min="8" max="8" width="18.425" customWidth="1"/>
+    <col min="8" max="8" width="19.25" style="8" customWidth="1"/>
     <col min="9" max="9" width="20.425" customWidth="1"/>
     <col min="10" max="10" width="21.8583333333333" customWidth="1"/>
     <col min="11" max="11" width="14.1416666666667" customWidth="1"/>
     <col min="12" max="12" width="17.425" customWidth="1"/>
     <col min="13" max="13" width="19.7083333333333" customWidth="1"/>
-    <col min="14" max="15" width="14.8583333333333" customWidth="1"/>
+    <col min="14" max="15" width="17.125" customWidth="1"/>
     <col min="16" max="16" width="17.2833333333333" customWidth="1"/>
     <col min="17" max="17" width="18.2833333333333" customWidth="1"/>
     <col min="18" max="18" width="20.8583333333333" customWidth="1"/>
@@ -1388,7 +1402,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -1444,7 +1458,7 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="I2" t="s">
@@ -1482,59 +1496,59 @@
       </c>
     </row>
     <row r="3" ht="54" spans="1:19">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="Q3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1545,7 +1559,7 @@
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D4">
@@ -1560,7 +1574,7 @@
       <c r="G4">
         <v>1.000111111</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="12" t="s">
         <v>51</v>
       </c>
       <c r="I4" t="s">
@@ -1569,29 +1583,29 @@
       <c r="K4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="7">
         <v>43415</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="7">
         <v>43415</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="7">
         <v>43415</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="7">
         <v>43415</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="7">
+        <v>43101.9999884259</v>
+      </c>
+      <c r="Q4" t="s">
         <v>54</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>55</v>
       </c>
       <c r="R4">
         <v>1123.0123456789</v>
       </c>
-      <c r="S4" s="8" t="s">
-        <v>56</v>
+      <c r="S4" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1599,7 +1613,7 @@
         <v>1000002</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>-100000</v>
@@ -1613,22 +1627,16 @@
       <c r="G5">
         <v>33333333333</v>
       </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" s="9">
+      <c r="L5" s="7">
         <v>43831.4999884259</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="7">
         <v>43831.4999884259</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="7">
         <v>43831.4999884259</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>43831.4999884259</v>
       </c>
       <c r="R5">
@@ -1640,7 +1648,7 @@
         <v>1000003</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6">
         <v>-32768</v>
@@ -1650,7 +1658,7 @@
       </c>
     </row>
     <row r="26" spans="15:15">
-      <c r="O26" s="8"/>
+      <c r="O26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1665,23 +1673,26 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
+  <cols>
+    <col min="4" max="4" width="16"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1689,13 +1700,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1703,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="D3" s="7">
+        <v>43101.9999884259</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1717,10 +1728,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1735,14 +1746,14 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1750,15 +1761,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1819,26 +1830,29 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <cols>
+    <col min="4" max="4" width="18.125"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1846,26 +1860,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" t="s">
         <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="5"/>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1876,47 +1890,68 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="6">
+        <v>222333</v>
       </c>
     </row>
   </sheetData>
@@ -1930,7 +1965,7 @@
   <sheetPr/>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
@@ -1941,13 +1976,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1969,13 +2004,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C3">
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1983,13 +2018,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1997,13 +2032,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2011,13 +2046,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2025,13 +2060,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2039,13 +2074,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C8">
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2053,13 +2088,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C9">
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add 3 level array 2.fix empty element bug 3.add 3 level array test case 4.update README.md
</commit_message>
<xml_diff>
--- a/testcase/Example.xlsx
+++ b/testcase/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23835" windowHeight="12615" activeTab="1"/>
+    <workbookView windowWidth="23835" windowHeight="12615" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -266,7 +266,7 @@
     <t>int_n_2</t>
   </si>
   <si>
-    <t>#int_n_n_n</t>
+    <t>int_n_n_n</t>
   </si>
   <si>
     <t>#</t>
@@ -281,10 +281,20 @@
     <t>int[][][]</t>
   </si>
   <si>
+    <t>111,112,113;121,122,123;131,132,133;
+211,212,213;221,222,223;231,232,233;
+311,312,313;321,322,323;331,332,333;</t>
+  </si>
+  <si>
     <t>1,2</t>
   </si>
   <si>
     <t>111,222;333,444</t>
+  </si>
+  <si>
+    <t>111,112,113;121,122,123;131,132,133
+211,212,213;221,222,223;231,232,233
+311,312,313;321,322,323;331,332,333</t>
   </si>
   <si>
     <t>11,22;55,66</t>
@@ -358,10 +368,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -386,19 +396,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -411,45 +412,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -471,11 +434,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,9 +473,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -508,13 +525,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -543,61 +553,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,121 +733,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,6 +744,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -791,41 +836,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -840,157 +850,160 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1370,7 +1383,7 @@
     <col min="5" max="5" width="18.425" customWidth="1"/>
     <col min="6" max="6" width="11.5666666666667" customWidth="1"/>
     <col min="7" max="7" width="12.7083333333333" customWidth="1"/>
-    <col min="8" max="8" width="19.25" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.25" style="9" customWidth="1"/>
     <col min="9" max="9" width="20.425" customWidth="1"/>
     <col min="10" max="10" width="21.8583333333333" customWidth="1"/>
     <col min="11" max="11" width="14.1416666666667" customWidth="1"/>
@@ -1405,7 +1418,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -1461,7 +1474,7 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="I2" t="s">
@@ -1499,59 +1512,59 @@
       </c>
     </row>
     <row r="3" ht="54" spans="1:19">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="11" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1562,7 +1575,7 @@
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D4">
@@ -1577,7 +1590,7 @@
       <c r="G4">
         <v>1.000111111</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="13" t="s">
         <v>51</v>
       </c>
       <c r="I4" t="s">
@@ -1586,19 +1599,19 @@
       <c r="K4" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="8">
         <v>43415</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="8">
         <v>43415</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="8">
         <v>43415</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="8">
         <v>43415</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="8">
         <v>43101.9999884259</v>
       </c>
       <c r="Q4" t="s">
@@ -1607,7 +1620,7 @@
       <c r="R4">
         <v>1123.0123456789</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1630,16 +1643,16 @@
       <c r="G5">
         <v>33333333333</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="8">
         <v>43831.4999884259</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="8">
         <v>43831.4999884259</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="8">
         <v>43831.4999884259</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="8">
         <v>43831.4999884259</v>
       </c>
       <c r="R5">
@@ -1661,7 +1674,7 @@
       </c>
     </row>
     <row r="26" spans="15:15">
-      <c r="O26" s="10"/>
+      <c r="O26" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1675,8 +1688,8 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -1722,7 +1735,7 @@
       <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="8">
         <v>43101.9999884259</v>
       </c>
     </row>
@@ -1832,14 +1845,15 @@
   <sheetPr/>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="4" max="4" width="18.125"/>
+    <col min="5" max="5" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1903,20 +1917,26 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" ht="81" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" ht="81" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1924,10 +1944,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1935,13 +1955,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1949,12 +1969,12 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="6">
+        <v>95</v>
+      </c>
+      <c r="D9" s="7">
         <v>222333</v>
       </c>
     </row>
@@ -1970,7 +1990,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -1980,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>69</v>
@@ -2008,13 +2028,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3">
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2022,13 +2042,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2036,7 +2056,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C5">
         <v>34</v>
@@ -2050,13 +2070,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C6">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2064,13 +2084,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2078,13 +2098,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C8">
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2092,13 +2112,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.add high type checker
</commit_message>
<xml_diff>
--- a/testcase/Example.xlsx
+++ b/testcase/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23835" windowHeight="12615" activeTab="3"/>
+    <workbookView windowWidth="24345" windowHeight="12615"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -369,9 +369,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -382,8 +382,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,7 +428,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,19 +441,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -436,15 +467,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,36 +496,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
@@ -496,14 +503,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -512,15 +512,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,31 +553,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,151 +721,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,56 +744,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -821,6 +771,54 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -838,9 +836,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,10 +850,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -862,139 +862,139 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1008,9 +1008,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1370,8 +1367,8 @@
   <sheetPr/>
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1515,56 +1512,56 @@
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1575,7 +1572,7 @@
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D4">
@@ -1590,7 +1587,7 @@
       <c r="G4">
         <v>1.000111111</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>51</v>
       </c>
       <c r="I4" t="s">
@@ -1620,7 +1617,7 @@
       <c r="R4">
         <v>1123.0123456789</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="S4" s="6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1674,7 +1671,7 @@
       </c>
     </row>
     <row r="26" spans="15:15">
-      <c r="O26" s="11"/>
+      <c r="O26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1845,8 +1842,8 @@
   <sheetPr/>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
version 2.6.1 add csharp export
</commit_message>
<xml_diff>
--- a/testcase/Example.xlsx
+++ b/testcase/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24345" windowHeight="12615"/>
+    <workbookView windowWidth="23925" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
   <si>
     <t>id</t>
   </si>
@@ -71,25 +71,28 @@
     <t>timestamparry</t>
   </si>
   <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>#string2</t>
+  </si>
+  <si>
+    <t>*int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
     <t>double</t>
-  </si>
-  <si>
-    <t>#string2</t>
-  </si>
-  <si>
-    <t>*int</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>float</t>
   </si>
   <si>
     <t>int[2]</t>
@@ -369,9 +372,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -382,39 +385,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,8 +399,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -441,19 +414,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,16 +437,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,15 +454,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,19 +499,35 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -553,187 +556,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,26 +750,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,8 +768,19 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,8 +803,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,27 +834,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -850,10 +853,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -862,134 +865,134 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1367,8 +1370,8 @@
   <sheetPr/>
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1469,19 +1472,19 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
         <v>11</v>
@@ -1496,73 +1499,73 @@
         <v>14</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="54" spans="1:19">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" ht="67.5" spans="1:19">
@@ -1570,10 +1573,10 @@
         <v>1000001</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4">
         <v>100000</v>
@@ -1588,13 +1591,13 @@
         <v>1.000111111</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L4" s="8">
         <v>43415</v>
@@ -1612,13 +1615,13 @@
         <v>43101.9999884259</v>
       </c>
       <c r="Q4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R4">
         <v>1123.0123456789</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1626,7 +1629,7 @@
         <v>1000002</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>-100000</v>
@@ -1661,7 +1664,7 @@
         <v>1000003</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6">
         <v>-32768</v>
@@ -1699,13 +1702,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1713,13 +1716,13 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1727,10 +1730,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D3" s="8">
         <v>43101.9999884259</v>
@@ -1741,10 +1744,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1766,7 +1769,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1774,15 +1777,15 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1855,19 +1858,19 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1875,26 +1878,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="5"/>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1902,16 +1905,16 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" ht="81" spans="1:5">
@@ -1919,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" ht="81" spans="1:5">
@@ -1927,13 +1930,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1941,10 +1944,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1952,13 +1955,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1966,10 +1969,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D9" s="7">
         <v>222333</v>
@@ -1997,13 +2000,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2025,13 +2028,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C3">
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2039,13 +2042,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2053,13 +2056,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C5">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2067,13 +2070,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C6">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2081,13 +2084,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2095,13 +2098,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C8">
         <v>43</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2109,13 +2112,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C9">
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 2.7.3 Add Name Translator and test case
</commit_message>
<xml_diff>
--- a/testcase/Example.xlsx
+++ b/testcase/Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23925" windowHeight="12690" activeTab="4"/>
+    <workbookView windowWidth="24225" windowHeight="12690" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
   <si>
     <t>AppType.ClientH |  AppType.ClientM | AppType.Gate | AppType.Logic</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
   <si>
     <t>int_2</t>
@@ -375,9 +378,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -385,110 +388,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -508,9 +407,106 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,7 +522,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -559,31 +562,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,43 +718,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,103 +736,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,6 +753,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -777,20 +789,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,17 +819,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -836,17 +834,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -856,10 +859,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -868,134 +871,134 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1863,8 +1866,8 @@
   <sheetPr/>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -1898,29 +1901,29 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="5"/>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1931,13 +1934,13 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" ht="81" spans="1:5">
@@ -1945,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" ht="81" spans="1:5">
@@ -1953,13 +1956,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1967,10 +1970,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1978,13 +1981,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1992,10 +1995,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" s="7">
         <v>222333</v>
@@ -2012,8 +2015,8 @@
   <sheetPr/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -2028,10 +2031,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
@@ -2056,13 +2059,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2070,13 +2073,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2084,7 +2087,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6">
         <v>34</v>
@@ -2098,13 +2101,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C7">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2112,13 +2115,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2126,13 +2129,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C9">
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2140,13 +2143,13 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C10">
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>